<commit_message>
Question Bank Update 10/25/2022
</commit_message>
<xml_diff>
--- a/Data/ClimateChange.xlsx
+++ b/Data/ClimateChange.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>Question</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">• Never                                                  • Sometimes                                      • Most of the time                            • Almost always </t>
   </si>
   <si>
-    <t>07/08/2022-07/15/2022</t>
+    <t>07/08/2022-07/15/2022 10/05/2022-10/12/2022</t>
   </si>
   <si>
     <t xml:space="preserve">How often do you do the following? Choose reusable water bottles, coffee cups, containers,  and utensils </t>
@@ -85,6 +85,9 @@
 </t>
   </si>
   <si>
+    <t>07/08/2022-07/15/2022</t>
+  </si>
+  <si>
     <t>How often do you spend time in nature with your child(ren)? This includes activities like going to a park, playing in a field, camping, hiking, visiting a beach, etc. This does not include activities like organized sports such as basketball or baseball.</t>
   </si>
   <si>
@@ -103,10 +106,13 @@
 • No                                                       • Prefer not to say  </t>
   </si>
   <si>
-    <t>06/02/2022-06/09/2022</t>
+    <t>06/02/2022-06/09/2022 10/05/2022-10/12/2022</t>
   </si>
   <si>
     <t>Do you worry about climate change and the impact it may have on the world?</t>
+  </si>
+  <si>
+    <t>06/02/2022-06/09/2022</t>
   </si>
   <si>
     <t xml:space="preserve">When thinking about climate change, do you have any of the feelings or experiences below?                                                       • I am hesitant to have more children 
@@ -138,7 +144,7 @@
 • Wildfires                                    • Not Listed (please specify)     • None of the above  </t>
   </si>
   <si>
-    <t>04/15/2022-04/20/2022</t>
+    <t>04/15/2022-04/20/2022 10/05/2022-10/12/2022</t>
   </si>
   <si>
     <t>How did these extreme weather events affect your family?</t>
@@ -149,6 +155,9 @@
   <si>
     <t>• Yes
 • No                                               • I don't know</t>
+  </si>
+  <si>
+    <t>04/15/2022-04/20/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Please indicate whether any of the following statements apply to your household.        There is trash and litter on the streets near my home </t>
@@ -167,6 +176,114 @@
   </si>
   <si>
     <t>How does the environment around your home (i.e., air quality, proximity to parks, etc.) affect your family?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Noise, smells, or dirt from cars, trucks or other road traffic </t>
+  </si>
+  <si>
+    <t>• 1                                                        • 2                                                        • 3                                                        • 4</t>
+  </si>
+  <si>
+    <t>10/05/2022-10/12/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Trash and litter on the streets near my home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Poorly maintained housing in my neighborhood </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Contaminated land (i.e. brownfields) or water (i.e. pollutants) near my home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Noise from aircrafts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Your neighbors’ noise or other activities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Undesirable business, institutional or industrial properties in my neighborhood </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+A lack of parks or green spaces </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Inadequate public transportation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+The amount of neighborhood crime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+The air quality around my home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+The quality of my drinking water </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Pesticides being applied near or around my home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
+Rate each on a scale of 1-5, with 5 meaning "most bothersome, disturbing, or annoying."
+Any other problems that you notice in your environment when you are at home (please specify) </t>
+  </si>
+  <si>
+    <t>How does the environment around your home (i.e. air quality, water quality, proximity to parks, etc.) affect your family?</t>
+  </si>
+  <si>
+    <t>Do you worry about the environment around your home and the impact it may have on your children?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Yes 
+• No 
+• Prefer not to say 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How often do you do the following? Reduce or eliminate travel by airplane </t>
+  </si>
+  <si>
+    <t>Do you involve your child(ren) in any activities that support environmental sustainability?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Never 
+• Rarely 
+• Sometimes 
+• Very often  
+• Always 
+</t>
+  </si>
+  <si>
+    <t>Please describe how you involve your child(ren) in activities that support environmental sustainability.</t>
+  </si>
+  <si>
+    <t>In what ways do you spend time in nature with your child(ren)?</t>
   </si>
 </sst>
 </file>
@@ -210,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border/>
     <border>
       <left style="thin">
@@ -254,11 +371,36 @@
         <color rgb="FFA6A6A6"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -278,11 +420,17 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -291,8 +439,24 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -870,7 +1034,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -896,10 +1060,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -930,15 +1094,15 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -964,15 +1128,15 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -998,15 +1162,15 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1032,15 +1196,15 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1066,15 +1230,15 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
+      <c r="E17" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1100,15 +1264,15 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>31</v>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1134,15 +1298,15 @@
     </row>
     <row r="19" ht="159.75" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1168,15 +1332,15 @@
     </row>
     <row r="20" ht="169.5" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1202,15 +1366,15 @@
     </row>
     <row r="21" ht="213.0" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1236,15 +1400,15 @@
     </row>
     <row r="22" ht="102.0" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1270,15 +1434,15 @@
     </row>
     <row r="23" ht="153.0" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1304,15 +1468,15 @@
     </row>
     <row r="24" ht="153.0" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1338,15 +1502,15 @@
     </row>
     <row r="25" ht="153.0" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1371,11 +1535,17 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" ht="102.0" customHeight="1">
-      <c r="A26" s="5"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1399,11 +1569,17 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" ht="169.5" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1427,11 +1603,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1455,11 +1637,17 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="1"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1483,11 +1671,17 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" ht="102.0" customHeight="1">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1511,11 +1705,17 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9"/>
+      <c r="A31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1539,11 +1739,17 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1567,11 +1773,17 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9"/>
+      <c r="A33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1595,11 +1807,17 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9"/>
+      <c r="A34" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -1623,11 +1841,17 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1651,11 +1875,17 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1679,11 +1909,17 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1707,11 +1943,17 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1735,11 +1977,17 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="A39" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1763,11 +2011,17 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="A40" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -1791,11 +2045,17 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="A41" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1819,11 +2079,17 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -1847,11 +2113,17 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="A43" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -1875,11 +2147,17 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="A44" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -1903,11 +2181,17 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="A45" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>

</xml_diff>

<commit_message>
11/16/2022 Question Bank Update
</commit_message>
<xml_diff>
--- a/Data/ClimateChange.xlsx
+++ b/Data/ClimateChange.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miEZxh8mqk2AHBQZbFv0lqyIvxjLg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhUHIfaDmXkmQM8hp7Jo5NeA3k7Sw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
   <si>
     <t>Question</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">• Never                                                  • Sometimes                                      • Most of the time                            • Almost always </t>
   </si>
   <si>
-    <t>07/08/2022-07/15/2022 10/05/2022-10/12/2022</t>
+    <t>07/08/2022-07/15/2022 10/05/2022-10/12/2022 11/08/2022-11/16/2022</t>
   </si>
   <si>
     <t xml:space="preserve">How often do you do the following? Choose reusable water bottles, coffee cups, containers,  and utensils </t>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">How often do you do the following? Choose eco-friendly brands when purchasing toiletries and/or cleaning products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How often do you do the following? Please specify any additional choices you make or activities that you engage in that support environmental sustainability </t>
+  </si>
+  <si>
+    <t>11/08/2022-11/16/2022</t>
   </si>
   <si>
     <t>Do you involve your child(ren) in climate change solutions (i.e. teaching them to recycle, bringing them to school via bike, providing them with disposable containers, etc.)</t>
@@ -106,7 +112,7 @@
 • No                                                       • Prefer not to say  </t>
   </si>
   <si>
-    <t>06/02/2022-06/09/2022 10/05/2022-10/12/2022</t>
+    <t>06/02/2022-06/09/2022 10/05/2022-10/12/2022 11/08/2022-11/16/2022</t>
   </si>
   <si>
     <t>Do you worry about climate change and the impact it may have on the world?</t>
@@ -144,7 +150,7 @@
 • Wildfires                                    • Not Listed (please specify)     • None of the above  </t>
   </si>
   <si>
-    <t>04/15/2022-04/20/2022 10/05/2022-10/12/2022</t>
+    <t>04/15/2022-04/20/2022 10/05/2022-10/12/2022 11/08/2022-11/16/2022</t>
   </si>
   <si>
     <t>How did these extreme weather events affect your family?</t>
@@ -186,7 +192,7 @@
     <t>• 1                                                        • 2                                                        • 3                                                        • 4</t>
   </si>
   <si>
-    <t>10/05/2022-10/12/2022</t>
+    <t>10/05/2022-10/12/2022 11/08/2022-11/16/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Thinking about the last 12 months or so, when you are at home, how much does each of the following bother, disturb, or annoy you?
@@ -1029,12 +1035,12 @@
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1060,15 +1066,15 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1102,7 +1108,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1128,10 +1134,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1165,12 +1171,12 @@
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1196,15 +1202,15 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1229,16 +1235,16 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1263,16 +1269,16 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>34</v>
+      <c r="A18" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1296,17 +1302,17 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" ht="159.75" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>35</v>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>37</v>
+      <c r="E19" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1330,17 +1336,17 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" ht="169.5" customHeight="1">
+    <row r="20" ht="159.75" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1364,17 +1370,17 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" ht="213.0" customHeight="1">
+    <row r="21" ht="169.5" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1398,17 +1404,17 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" ht="102.0" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>40</v>
+    <row r="22" ht="213.0" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1432,17 +1438,17 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" ht="153.0" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>41</v>
+    <row r="23" ht="102.0" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1468,15 +1474,15 @@
     </row>
     <row r="24" ht="153.0" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1502,15 +1508,15 @@
     </row>
     <row r="25" ht="153.0" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1534,17 +1540,17 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" ht="102.0" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="26" ht="153.0" customHeight="1">
+      <c r="A26" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="4" t="s">
-        <v>46</v>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1568,17 +1574,17 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" ht="169.5" customHeight="1">
+    <row r="27" ht="102.0" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="8"/>
       <c r="E27" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1602,17 +1608,17 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>48</v>
+    <row r="28" ht="169.5" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="8"/>
       <c r="E28" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1638,15 +1644,15 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="8"/>
       <c r="E29" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1670,17 +1676,17 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" ht="102.0" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>50</v>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="8"/>
       <c r="E30" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1704,17 +1710,17 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="9" t="s">
-        <v>51</v>
+    <row r="31" ht="102.0" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>52</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>45</v>
+      <c r="B31" s="4" t="s">
+        <v>47</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="10" t="s">
-        <v>46</v>
+      <c r="C31" s="1"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1740,15 +1746,15 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -1774,15 +1780,15 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
       <c r="E33" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1807,16 +1813,16 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="13" t="s">
-        <v>54</v>
+      <c r="A34" s="9" t="s">
+        <v>55</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>45</v>
+      <c r="B34" s="10" t="s">
+        <v>47</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="14" t="s">
-        <v>46</v>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1841,16 +1847,16 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>55</v>
+      <c r="A35" s="13" t="s">
+        <v>56</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>45</v>
+      <c r="B35" s="14" t="s">
+        <v>47</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="17" t="s">
-        <v>46</v>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1876,15 +1882,15 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1910,15 +1916,15 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
       <c r="E37" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1944,15 +1950,15 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1978,15 +1984,15 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
       <c r="E39" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2012,15 +2018,15 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>30</v>
+      <c r="B40" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
       <c r="E40" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2046,15 +2052,15 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -2083,12 +2089,12 @@
         <v>63</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2114,15 +2120,15 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2151,12 +2157,12 @@
         <v>66</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2182,15 +2188,15 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -2215,11 +2221,17 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="A46" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -29374,6 +29386,34 @@
       <c r="Y1015" s="2"/>
       <c r="Z1015" s="2"/>
     </row>
+    <row r="1016" ht="15.75" customHeight="1">
+      <c r="A1016" s="2"/>
+      <c r="B1016" s="2"/>
+      <c r="C1016" s="2"/>
+      <c r="D1016" s="2"/>
+      <c r="E1016" s="2"/>
+      <c r="F1016" s="2"/>
+      <c r="G1016" s="2"/>
+      <c r="H1016" s="2"/>
+      <c r="I1016" s="2"/>
+      <c r="J1016" s="2"/>
+      <c r="K1016" s="2"/>
+      <c r="L1016" s="2"/>
+      <c r="M1016" s="2"/>
+      <c r="N1016" s="2"/>
+      <c r="O1016" s="2"/>
+      <c r="P1016" s="2"/>
+      <c r="Q1016" s="2"/>
+      <c r="R1016" s="2"/>
+      <c r="S1016" s="2"/>
+      <c r="T1016" s="2"/>
+      <c r="U1016" s="2"/>
+      <c r="V1016" s="2"/>
+      <c r="W1016" s="2"/>
+      <c r="X1016" s="2"/>
+      <c r="Y1016" s="2"/>
+      <c r="Z1016" s="2"/>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>